<commit_message>
started to write the simulation parameters
</commit_message>
<xml_diff>
--- a/public/BPH060225.xlsx
+++ b/public/BPH060225.xlsx
@@ -10,8 +10,8 @@
   <sheets>
     <sheet name="info ini" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="calcul" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="field" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="BPH" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="BPH" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="field" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -118,9 +118,6 @@
     <t xml:space="preserve">TOTAL TREATMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">TOTAL YIELD</t>
-  </si>
-  <si>
     <t xml:space="preserve">week</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Final yield (t/ha):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL YIELD</t>
   </si>
 </sst>
 </file>
@@ -269,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -320,13 +320,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="medium"/>
@@ -337,14 +330,14 @@
       <left style="medium"/>
       <right style="medium"/>
       <top/>
-      <bottom/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom style="medium"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -375,7 +368,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -468,18 +461,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -492,11 +473,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,7 +481,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,6 +495,18 @@
     </xf>
     <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -857,10 +846,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0351668169522092"/>
-          <c:y val="0.0439907038512616"/>
-          <c:w val="0.915883034909185"/>
-          <c:h val="0.777888446215139"/>
+          <c:x val="0.035168327035383"/>
+          <c:y val="0.0439943554411887"/>
+          <c:w val="0.915836482308485"/>
+          <c:h val="0.77778700091309"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1002,34 +991,34 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.2802</c:v>
+                  <c:v>110.338014971209</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0094626815965</c:v>
+                  <c:v>118.168427712176</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.055583804632</c:v>
+                  <c:v>121.359710311417</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.4430420015479</c:v>
+                  <c:v>116.755175091851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.5080416586947</c:v>
+                  <c:v>99.7500177775418</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>139.982876349511</c:v>
+                  <c:v>31.5791331003943</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>252.790246769528</c:v>
+                  <c:v>17.7296775505161</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>418.349573783419</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>727.67088775234</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1289.88212741324</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1172,34 +1161,34 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6875</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6328125</c:v>
+                  <c:v>23.4375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2373046875</c:v>
+                  <c:v>29.296875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0889892578125</c:v>
+                  <c:v>36.62109375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0333709716796875</c:v>
+                  <c:v>13.73291015625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0417137145996094</c:v>
+                  <c:v>17.1661376953125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0156426429748535</c:v>
+                  <c:v>19.6467814816582</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.00586599111557007</c:v>
+                  <c:v>6.32014817640527</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.00219974666833877</c:v>
+                  <c:v>2.23258164550057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,34 +1331,34 @@
                   <c:v>4.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.662</c:v>
+                  <c:v>5.324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4641</c:v>
+                  <c:v>5.8564</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.805255</c:v>
+                  <c:v>6.44204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44289025</c:v>
+                  <c:v>7.086244</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2435896375</c:v>
+                  <c:v>7.79486840000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.133974300625</c:v>
+                  <c:v>4.28717762</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1473717306875</c:v>
+                  <c:v>4.715895382</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0810544518781251</c:v>
+                  <c:v>5.18748492020001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0445799485329688</c:v>
+                  <c:v>2.85311670611</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0245189716931328</c:v>
+                  <c:v>1.5692141883605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1384,8 +1373,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="98460587"/>
-        <c:axId val="47050420"/>
+        <c:axId val="40387837"/>
+        <c:axId val="18471408"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1516,19 +1505,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1537,7 +1526,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -1558,11 +1547,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="91274870"/>
-        <c:axId val="15761730"/>
+        <c:axId val="15169437"/>
+        <c:axId val="67726273"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98460587"/>
+        <c:axId val="40387837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,7 +1584,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47050420"/>
+        <c:crossAx val="18471408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1603,7 +1592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47050420"/>
+        <c:axId val="18471408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1644,12 +1633,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98460587"/>
+        <c:crossAx val="40387837"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="91274870"/>
+        <c:axId val="15169437"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,14 +1671,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15761730"/>
+        <c:crossAx val="67726273"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15761730"/>
+        <c:axId val="67726273"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1721,7 +1710,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91274870"/>
+        <c:crossAx val="15169437"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1787,10 +1776,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.116615067079463"/>
-          <c:y val="0.0369458128078818"/>
-          <c:w val="0.883226164959911"/>
-          <c:h val="0.808092892329346"/>
+          <c:x val="0.116619695947287"/>
+          <c:y val="0.0369484129776902"/>
+          <c:w val="0.883181836224348"/>
+          <c:h val="0.808009008374974"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1926,40 +1915,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.454545454545455</c:v>
+                  <c:v>0.151515151515152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88888888888889</c:v>
+                  <c:v>0.282828282828283</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.31749084848485</c:v>
+                  <c:v>0.390806662129937</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.74048902517915</c:v>
+                  <c:v>0.473330730228935</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.15386603712817</c:v>
+                  <c:v>0.530370629800604</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.54982527970438</c:v>
+                  <c:v>0.565684043583844</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.91362885747219</c:v>
+                  <c:v>0.589434401914201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2167440755588</c:v>
+                  <c:v>0.648120825079113</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.38902776975862</c:v>
+                  <c:v>0.713018039531713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.34301108378896</c:v>
+                  <c:v>0.782141256045338</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.86878898355414</c:v>
+                  <c:v>0.849244270538761</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.43558661976165</c:v>
+                  <c:v>0.83813315942765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2144,11 +2133,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="63833707"/>
-        <c:axId val="88052572"/>
+        <c:axId val="34448202"/>
+        <c:axId val="17286583"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63833707"/>
+        <c:axId val="34448202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2170,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88052572"/>
+        <c:crossAx val="17286583"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2189,7 +2178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88052572"/>
+        <c:axId val="17286583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +2218,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63833707"/>
+        <c:crossAx val="34448202"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2735,11 +2724,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="42669188"/>
-        <c:axId val="96520098"/>
+        <c:axId val="51858453"/>
+        <c:axId val="17536896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42669188"/>
+        <c:axId val="51858453"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,7 +2761,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96520098"/>
+        <c:crossAx val="17536896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2780,7 +2769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96520098"/>
+        <c:axId val="17536896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2820,7 +2809,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42669188"/>
+        <c:crossAx val="51858453"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2884,9 +2873,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>67680</xdr:colOff>
+      <xdr:colOff>67320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2895,7 +2884,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="20975400" y="317520"/>
-        <a:ext cx="8383680" cy="4336920"/>
+        <a:ext cx="8383320" cy="4336560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2914,9 +2903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
+      <xdr:colOff>95040</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2925,7 +2914,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="20317320" y="4821480"/>
-        <a:ext cx="9069480" cy="5115240"/>
+        <a:ext cx="9069120" cy="5114880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2949,9 +2938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:colOff>40320</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2960,7 +2949,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="14086080" y="163800"/>
-        <a:ext cx="5914440" cy="4738320"/>
+        <a:ext cx="5914080" cy="4737960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2979,9 +2968,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>147240</xdr:colOff>
+      <xdr:colOff>146880</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>341640</xdr:rowOff>
+      <xdr:rowOff>341280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2991,7 +2980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14615640" y="257040"/>
-          <a:ext cx="5491440" cy="4456440"/>
+          <a:ext cx="5491080" cy="4456080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3206,7 +3195,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3373,8 +3362,8 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3504,15 +3493,15 @@
         <v>0</v>
       </c>
       <c r="N2" s="20" t="n">
-        <f aca="false">300</f>
-        <v>300</v>
+        <f aca="false">100</f>
+        <v>100</v>
       </c>
       <c r="O2" s="19" t="n">
         <v>0</v>
       </c>
       <c r="P2" s="21" t="n">
         <f aca="false">N2/300</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="Q2" s="21" t="n">
         <f aca="false">N2*O2*5/(100*300)</f>
@@ -3579,7 +3568,7 @@
       </c>
       <c r="N3" s="16" t="n">
         <f aca="false">IF((N2-(B3/15))&gt;0,N2-(B3/15),0)</f>
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="O3" s="19" t="n">
         <f aca="false">A3*100/11</f>
@@ -3587,11 +3576,11 @@
       </c>
       <c r="P3" s="19" t="n">
         <f aca="false">N3/300</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="Q3" s="19" t="n">
         <f aca="false">N3*O3*5/(100*300)</f>
-        <v>0.454545454545455</v>
+        <v>0.151515151515152</v>
       </c>
       <c r="R3" s="11" t="n">
         <f aca="false">BPH!C3</f>
@@ -3655,7 +3644,7 @@
       </c>
       <c r="N4" s="16" t="n">
         <f aca="false">IF((N3-(B4/15))&gt;0,N3-(B4/15),0)</f>
-        <v>293.333333333333</v>
+        <v>93.3333333333333</v>
       </c>
       <c r="O4" s="19" t="n">
         <f aca="false">A4*100/11</f>
@@ -3663,15 +3652,15 @@
       </c>
       <c r="P4" s="19" t="n">
         <f aca="false">N4/300</f>
-        <v>0.977777777777778</v>
+        <v>0.311111111111111</v>
       </c>
       <c r="Q4" s="19" t="n">
         <f aca="false">N4*O4*5/(100*300)</f>
-        <v>0.88888888888889</v>
+        <v>0.282828282828283</v>
       </c>
       <c r="R4" s="11" t="n">
         <f aca="false">BPH!C4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="16"/>
       <c r="T4" s="11" t="n">
@@ -3685,7 +3674,7 @@
       </c>
       <c r="B5" s="16" t="n">
         <f aca="false">C5+D5</f>
-        <v>52.2802</v>
+        <v>110.338014971209</v>
       </c>
       <c r="C5" s="17" t="n">
         <f aca="false">C4*(1-M4)*IF(SUM($R$2:R4)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
@@ -3693,7 +3682,7 @@
       </c>
       <c r="D5" s="16" t="n">
         <f aca="false">D4*(1-M4)*IF(SUM($R$2,R4)=0,'info ini'!B$4,'info ini'!B$5)*IF(R4=1,'info ini'!B$7,1)+9.8</f>
-        <v>42.0704</v>
+        <v>100.128214971209</v>
       </c>
       <c r="E5" s="16" t="n">
         <f aca="false">F4*'info ini'!C$4</f>
@@ -3701,11 +3690,11 @@
       </c>
       <c r="F5" s="18" t="n">
         <f aca="false">IF(R4=1,'info ini'!$C$7,1)*F4*IF(K4=L4,'info ini'!$C$4,(('info ini'!$C$4-1)*L4/K4)+1)</f>
-        <v>4.5</v>
+        <v>15</v>
       </c>
       <c r="G5" s="16" t="n">
         <f aca="false">F5*'info ini'!$C$6</f>
-        <v>4.95</v>
+        <v>16.5</v>
       </c>
       <c r="H5" s="16" t="n">
         <f aca="false">I4*'info ini'!D$4</f>
@@ -3713,27 +3702,27 @@
       </c>
       <c r="I5" s="18" t="n">
         <f aca="false">IF(R4=1,'info ini'!$D$7,1)*I4*'info ini'!$D$4</f>
-        <v>2.662</v>
+        <v>5.324</v>
       </c>
       <c r="J5" s="16" t="n">
         <f aca="false">I5*'info ini'!$D$6</f>
-        <v>6.655</v>
+        <v>13.31</v>
       </c>
       <c r="K5" s="16" t="n">
         <f aca="false">J5+G5</f>
-        <v>11.605</v>
+        <v>29.81</v>
       </c>
       <c r="L5" s="18" t="n">
         <f aca="false">IF((G5+J5)&lt;B5,(G5+J5),B5)</f>
-        <v>11.605</v>
+        <v>29.81</v>
       </c>
       <c r="M5" s="19" t="n">
         <f aca="false">IF(B5=0,0,L5/B5)</f>
-        <v>0.221976962597695</v>
+        <v>0.270169805100975</v>
       </c>
       <c r="N5" s="16" t="n">
         <f aca="false">IF((N4-(B5/15))&gt;0,N4-(B5/15),0)</f>
-        <v>289.847986666666</v>
+        <v>85.9774656685861</v>
       </c>
       <c r="O5" s="19" t="n">
         <f aca="false">A5*100/11</f>
@@ -3741,15 +3730,15 @@
       </c>
       <c r="P5" s="19" t="n">
         <f aca="false">N5/300</f>
-        <v>0.966159955555554</v>
+        <v>0.28659155222862</v>
       </c>
       <c r="Q5" s="19" t="n">
         <f aca="false">N5*O5*5/(100*300)</f>
-        <v>1.31749084848485</v>
+        <v>0.390806662129937</v>
       </c>
       <c r="R5" s="11" t="n">
         <f aca="false">BPH!C5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="16"/>
       <c r="T5" s="11" t="n">
@@ -3763,55 +3752,55 @@
       </c>
       <c r="B6" s="16" t="n">
         <f aca="false">C6+D6</f>
-        <v>40.0094626815965</v>
+        <v>118.168427712177</v>
       </c>
       <c r="C6" s="17" t="n">
         <f aca="false">C5*(1-M5)*IF(SUM($R$2:R5)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>14.4982272930861</v>
+        <v>10.1849032339993</v>
       </c>
       <c r="D6" s="16" t="n">
         <f aca="false">D5*(1-M5)*IF(SUM($R$2,R5)=0,'info ini'!B$4,'info ini'!B$5)*IF(R5=1,'info ini'!B$7,1)+9.8</f>
-        <v>25.5112353885104</v>
+        <v>107.983524478177</v>
       </c>
       <c r="E6" s="16" t="n">
         <f aca="false">F5*'info ini'!C$4</f>
-        <v>5.625</v>
+        <v>18.75</v>
       </c>
       <c r="F6" s="18" t="n">
         <f aca="false">IF(R5=1,'info ini'!$C$7,1)*F5*IF(K5=L5,'info ini'!$C$4,(('info ini'!$C$4-1)*L5/K5)+1)</f>
-        <v>1.6875</v>
+        <v>18.75</v>
       </c>
       <c r="G6" s="16" t="n">
         <f aca="false">F6*'info ini'!$C$6</f>
-        <v>1.85625</v>
+        <v>20.625</v>
       </c>
       <c r="H6" s="16" t="n">
         <f aca="false">I5*'info ini'!D$4</f>
-        <v>2.9282</v>
+        <v>5.8564</v>
       </c>
       <c r="I6" s="18" t="n">
         <f aca="false">IF(R5=1,'info ini'!$D$7,1)*I5*'info ini'!$D$4</f>
-        <v>1.4641</v>
+        <v>5.8564</v>
       </c>
       <c r="J6" s="16" t="n">
         <f aca="false">I6*'info ini'!$D$6</f>
-        <v>3.66025</v>
+        <v>14.641</v>
       </c>
       <c r="K6" s="16" t="n">
         <f aca="false">J6+G6</f>
-        <v>5.5165</v>
+        <v>35.266</v>
       </c>
       <c r="L6" s="18" t="n">
         <f aca="false">IF((G6+J6)&lt;B6,(G6+J6),B6)</f>
-        <v>5.5165</v>
+        <v>35.266</v>
       </c>
       <c r="M6" s="19" t="n">
         <f aca="false">IF(B6=0,0,L6/B6)</f>
-        <v>0.137879882164413</v>
+        <v>0.298438429644656</v>
       </c>
       <c r="N6" s="16" t="n">
         <f aca="false">IF((N5-(B6/15))&gt;0,N5-(B6/15),0)</f>
-        <v>287.18068915456</v>
+        <v>78.0995704877743</v>
       </c>
       <c r="O6" s="19" t="n">
         <f aca="false">A6*100/11</f>
@@ -3819,15 +3808,15 @@
       </c>
       <c r="P6" s="19" t="n">
         <f aca="false">N6/300</f>
-        <v>0.957268963848533</v>
+        <v>0.260331901625914</v>
       </c>
       <c r="Q6" s="19" t="n">
         <f aca="false">N6*O6*5/(100*300)</f>
-        <v>1.74048902517915</v>
+        <v>0.473330730228935</v>
       </c>
       <c r="R6" s="11" t="n">
         <f aca="false">BPH!C6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" s="16"/>
       <c r="T6" s="11" t="n">
@@ -3841,55 +3830,55 @@
       </c>
       <c r="B7" s="16" t="n">
         <f aca="false">C7+D7</f>
-        <v>43.055583804632</v>
+        <v>121.359710311419</v>
       </c>
       <c r="C7" s="17" t="n">
         <f aca="false">C6*(1-M6)*IF(SUM($R$2:R6)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>22.6985841601805</v>
+        <v>9.77475118706077</v>
       </c>
       <c r="D7" s="16" t="n">
         <f aca="false">D6*(1-M6)*IF(SUM($R$2,R6)=0,'info ini'!B$4,'info ini'!B$5)*IF(R6=1,'info ini'!B$7,1)+9.8</f>
-        <v>20.3569996444515</v>
+        <v>111.584959124358</v>
       </c>
       <c r="E7" s="16" t="n">
         <f aca="false">F6*'info ini'!C$4</f>
-        <v>2.109375</v>
+        <v>23.4375</v>
       </c>
       <c r="F7" s="18" t="n">
         <f aca="false">IF(R6=1,'info ini'!$C$7,1)*F6*IF(K6=L6,'info ini'!$C$4,(('info ini'!$C$4-1)*L6/K6)+1)</f>
-        <v>0.6328125</v>
+        <v>23.4375</v>
       </c>
       <c r="G7" s="16" t="n">
         <f aca="false">F7*'info ini'!$C$6</f>
-        <v>0.69609375</v>
+        <v>25.78125</v>
       </c>
       <c r="H7" s="16" t="n">
         <f aca="false">I6*'info ini'!D$4</f>
-        <v>1.61051</v>
+        <v>6.44204</v>
       </c>
       <c r="I7" s="18" t="n">
         <f aca="false">IF(R6=1,'info ini'!$D$7,1)*I6*'info ini'!$D$4</f>
-        <v>0.805255</v>
+        <v>6.44204</v>
       </c>
       <c r="J7" s="16" t="n">
         <f aca="false">I7*'info ini'!$D$6</f>
-        <v>2.0131375</v>
+        <v>16.1051</v>
       </c>
       <c r="K7" s="16" t="n">
         <f aca="false">J7+G7</f>
-        <v>2.70923125</v>
+        <v>41.88635</v>
       </c>
       <c r="L7" s="18" t="n">
         <f aca="false">IF((G7+J7)&lt;B7,(G7+J7),B7)</f>
-        <v>2.70923125</v>
+        <v>41.88635</v>
       </c>
       <c r="M7" s="19" t="n">
         <f aca="false">IF(B7=0,0,L7/B7)</f>
-        <v>0.062924039360222</v>
+        <v>0.345142138956301</v>
       </c>
       <c r="N7" s="16" t="n">
         <f aca="false">IF((N6-(B7/15))&gt;0,N6-(B7/15),0)</f>
-        <v>284.310316900918</v>
+        <v>70.0089231336797</v>
       </c>
       <c r="O7" s="19" t="n">
         <f aca="false">A7*100/11</f>
@@ -3897,15 +3886,15 @@
       </c>
       <c r="P7" s="19" t="n">
         <f aca="false">N7/300</f>
-        <v>0.947701056336393</v>
+        <v>0.233363077112266</v>
       </c>
       <c r="Q7" s="19" t="n">
         <f aca="false">N7*O7*5/(100*300)</f>
-        <v>2.15386603712817</v>
+        <v>0.530370629800604</v>
       </c>
       <c r="R7" s="11" t="n">
         <f aca="false">BPH!C7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="16"/>
       <c r="T7" s="11" t="n">
@@ -3919,55 +3908,55 @@
       </c>
       <c r="B8" s="16" t="n">
         <f aca="false">C8+D8</f>
-        <v>57.4430420015479</v>
+        <v>116.755175091853</v>
       </c>
       <c r="C8" s="17" t="n">
         <f aca="false">C7*(1-M7)*IF(SUM($R$2:R7)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>38.4865356027152</v>
+        <v>8.77743735715458</v>
       </c>
       <c r="D8" s="16" t="n">
         <f aca="false">D7*(1-M7)*IF(SUM($R$2,R7)=0,'info ini'!B$4,'info ini'!B$5)*IF(R7=1,'info ini'!B$7,1)+9.8</f>
-        <v>18.9565063988326</v>
+        <v>107.977737734698</v>
       </c>
       <c r="E8" s="16" t="n">
         <f aca="false">F7*'info ini'!C$4</f>
-        <v>0.791015625</v>
+        <v>29.296875</v>
       </c>
       <c r="F8" s="18" t="n">
         <f aca="false">IF(R7=1,'info ini'!$C$7,1)*F7*IF(K7=L7,'info ini'!$C$4,(('info ini'!$C$4-1)*L7/K7)+1)</f>
-        <v>0.2373046875</v>
+        <v>29.296875</v>
       </c>
       <c r="G8" s="16" t="n">
         <f aca="false">F8*'info ini'!$C$6</f>
-        <v>0.26103515625</v>
+        <v>32.2265625</v>
       </c>
       <c r="H8" s="16" t="n">
         <f aca="false">I7*'info ini'!D$4</f>
-        <v>0.885780500000001</v>
+        <v>7.086244</v>
       </c>
       <c r="I8" s="18" t="n">
         <f aca="false">IF(R7=1,'info ini'!$D$7,1)*I7*'info ini'!$D$4</f>
-        <v>0.44289025</v>
+        <v>7.086244</v>
       </c>
       <c r="J8" s="16" t="n">
         <f aca="false">I8*'info ini'!$D$6</f>
-        <v>1.107225625</v>
+        <v>17.71561</v>
       </c>
       <c r="K8" s="16" t="n">
         <f aca="false">J8+G8</f>
-        <v>1.36826078125</v>
+        <v>49.9421725</v>
       </c>
       <c r="L8" s="18" t="n">
         <f aca="false">IF((G8+J8)&lt;B8,(G8+J8),B8)</f>
-        <v>1.36826078125</v>
+        <v>49.9421725</v>
       </c>
       <c r="M8" s="19" t="n">
         <f aca="false">IF(B8=0,0,L8/B8)</f>
-        <v>0.023819434583794</v>
+        <v>0.427751253515827</v>
       </c>
       <c r="N8" s="16" t="n">
         <f aca="false">IF((N7-(B8/15))&gt;0,N7-(B8/15),0)</f>
-        <v>280.480780767481</v>
+        <v>62.2252447942228</v>
       </c>
       <c r="O8" s="19" t="n">
         <f aca="false">A8*100/11</f>
@@ -3975,15 +3964,15 @@
       </c>
       <c r="P8" s="19" t="n">
         <f aca="false">N8/300</f>
-        <v>0.934935935891604</v>
+        <v>0.207417482647409</v>
       </c>
       <c r="Q8" s="19" t="n">
         <f aca="false">N8*O8*5/(100*300)</f>
-        <v>2.54982527970438</v>
+        <v>0.565684043583844</v>
       </c>
       <c r="R8" s="11" t="n">
         <f aca="false">BPH!C8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="16"/>
       <c r="T8" s="11" t="n">
@@ -3997,55 +3986,55 @@
       </c>
       <c r="B9" s="16" t="n">
         <f aca="false">C9+D9</f>
-        <v>86.5080416586947</v>
+        <v>99.7500177775444</v>
       </c>
       <c r="C9" s="17" t="n">
         <f aca="false">C8*(1-M8)*IF(SUM($R$2:R8)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>67.8256545540251</v>
+        <v>6.93065588346658</v>
       </c>
       <c r="D9" s="16" t="n">
         <f aca="false">D8*(1-M8)*IF(SUM($R$2,R8)=0,'info ini'!B$4,'info ini'!B$5)*IF(R8=1,'info ini'!B$7,1)+9.8</f>
-        <v>18.6823871046696</v>
+        <v>92.8193618940778</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">F8*'info ini'!C$4</f>
-        <v>0.296630859375</v>
+        <v>36.62109375</v>
       </c>
       <c r="F9" s="18" t="n">
         <f aca="false">IF(R8=1,'info ini'!$C$7,1)*F8*IF(K8=L8,'info ini'!$C$4,(('info ini'!$C$4-1)*L8/K8)+1)</f>
-        <v>0.0889892578125</v>
+        <v>36.62109375</v>
       </c>
       <c r="G9" s="16" t="n">
         <f aca="false">F9*'info ini'!$C$6</f>
-        <v>0.09788818359375</v>
+        <v>40.283203125</v>
       </c>
       <c r="H9" s="16" t="n">
         <f aca="false">I8*'info ini'!D$4</f>
-        <v>0.487179275</v>
+        <v>7.79486840000001</v>
       </c>
       <c r="I9" s="18" t="n">
         <f aca="false">IF(R8=1,'info ini'!$D$7,1)*I8*'info ini'!$D$4</f>
-        <v>0.2435896375</v>
+        <v>7.79486840000001</v>
       </c>
       <c r="J9" s="16" t="n">
         <f aca="false">I9*'info ini'!$D$6</f>
-        <v>0.60897409375</v>
+        <v>19.487171</v>
       </c>
       <c r="K9" s="16" t="n">
         <f aca="false">J9+G9</f>
-        <v>0.70686227734375</v>
+        <v>59.770374125</v>
       </c>
       <c r="L9" s="18" t="n">
         <f aca="false">IF((G9+J9)&lt;B9,(G9+J9),B9)</f>
-        <v>0.70686227734375</v>
+        <v>59.770374125</v>
       </c>
       <c r="M9" s="19" t="n">
         <f aca="false">IF(B9=0,0,L9/B9)</f>
-        <v>0.00817105859513704</v>
+        <v>0.599201638823722</v>
       </c>
       <c r="N9" s="16" t="n">
         <f aca="false">IF((N8-(B9/15))&gt;0,N8-(B9/15),0)</f>
-        <v>274.713577990235</v>
+        <v>55.5752436090532</v>
       </c>
       <c r="O9" s="19" t="n">
         <f aca="false">A9*100/11</f>
@@ -4053,11 +4042,11 @@
       </c>
       <c r="P9" s="19" t="n">
         <f aca="false">N9/300</f>
-        <v>0.915711926634116</v>
+        <v>0.185250812030177</v>
       </c>
       <c r="Q9" s="19" t="n">
         <f aca="false">N9*O9*5/(100*300)</f>
-        <v>2.91362885747219</v>
+        <v>0.589434401914201</v>
       </c>
       <c r="R9" s="11" t="n">
         <f aca="false">BPH!C9</f>
@@ -4075,55 +4064,55 @@
       </c>
       <c r="B10" s="16" t="n">
         <f aca="false">C10+D10</f>
-        <v>139.982876349511</v>
+        <v>31.5791331003956</v>
       </c>
       <c r="C10" s="17" t="n">
         <f aca="false">C9*(1-M9)*IF(SUM($R$2:R9)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>121.288604881539</v>
+        <v>3.92224599675998</v>
       </c>
       <c r="D10" s="16" t="n">
         <f aca="false">D9*(1-M9)*IF(SUM($R$2,R9)=0,'info ini'!B$4,'info ini'!B$5)*IF(R9=1,'info ini'!B$7,1)+9.8</f>
-        <v>18.6942714679714</v>
+        <v>27.6568871036356</v>
       </c>
       <c r="E10" s="16" t="n">
         <f aca="false">F9*'info ini'!C$4</f>
-        <v>0.111236572265625</v>
+        <v>45.7763671875</v>
       </c>
       <c r="F10" s="18" t="n">
         <f aca="false">IF(R9=1,'info ini'!$C$7,1)*F9*IF(K9=L9,'info ini'!$C$4,(('info ini'!$C$4-1)*L9/K9)+1)</f>
-        <v>0.0333709716796875</v>
+        <v>13.73291015625</v>
       </c>
       <c r="G10" s="16" t="n">
         <f aca="false">F10*'info ini'!$C$6</f>
-        <v>0.0367080688476562</v>
+        <v>15.106201171875</v>
       </c>
       <c r="H10" s="16" t="n">
         <f aca="false">I9*'info ini'!D$4</f>
-        <v>0.26794860125</v>
+        <v>8.57435524000001</v>
       </c>
       <c r="I10" s="18" t="n">
         <f aca="false">IF(R9=1,'info ini'!$D$7,1)*I9*'info ini'!$D$4</f>
-        <v>0.133974300625</v>
+        <v>4.28717762</v>
       </c>
       <c r="J10" s="16" t="n">
         <f aca="false">I10*'info ini'!$D$6</f>
-        <v>0.3349357515625</v>
+        <v>10.71794405</v>
       </c>
       <c r="K10" s="16" t="n">
         <f aca="false">J10+G10</f>
-        <v>0.371643820410157</v>
+        <v>25.824145221875</v>
       </c>
       <c r="L10" s="18" t="n">
         <f aca="false">IF((G10+J10)&lt;B10,(G10+J10),B10)</f>
-        <v>0.371643820410157</v>
+        <v>25.824145221875</v>
       </c>
       <c r="M10" s="19" t="n">
         <f aca="false">IF(B10=0,0,L10/B10)</f>
-        <v>0.00265492344565226</v>
+        <v>0.817759789028265</v>
       </c>
       <c r="N10" s="16" t="n">
         <f aca="false">IF((N9-(B10/15))&gt;0,N9-(B10/15),0)</f>
-        <v>265.381386233601</v>
+        <v>53.4699680690268</v>
       </c>
       <c r="O10" s="19" t="n">
         <f aca="false">A10*100/11</f>
@@ -4131,11 +4120,11 @@
       </c>
       <c r="P10" s="19" t="n">
         <f aca="false">N10/300</f>
-        <v>0.88460462077867</v>
+        <v>0.178233226896756</v>
       </c>
       <c r="Q10" s="19" t="n">
         <f aca="false">N10*O10*5/(100*300)</f>
-        <v>3.2167440755588</v>
+        <v>0.648120825079113</v>
       </c>
       <c r="R10" s="11" t="n">
         <f aca="false">BPH!C10</f>
@@ -4153,55 +4142,55 @@
       </c>
       <c r="B11" s="16" t="n">
         <f aca="false">C11+D11</f>
-        <v>252.790246769528</v>
+        <v>17.729677550518</v>
       </c>
       <c r="C11" s="17" t="n">
         <f aca="false">C10*(1-M10)*IF(SUM($R$2:R10)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>217.939867257348</v>
+        <v>1.15781985682966</v>
       </c>
       <c r="D11" s="16" t="n">
         <f aca="false">D10*(1-M10)*IF(SUM($R$2,R10)=0,'info ini'!B$4,'info ini'!B$5)*IF(R10=1,'info ini'!B$7,1)+9.8</f>
-        <v>34.8503795121807</v>
+        <v>16.5718576936883</v>
       </c>
       <c r="E11" s="16" t="n">
         <f aca="false">F10*'info ini'!C$4</f>
-        <v>0.0417137145996094</v>
+        <v>17.1661376953125</v>
       </c>
       <c r="F11" s="18" t="n">
         <f aca="false">IF(R10=1,'info ini'!$C$7,1)*F10*IF(K10=L10,'info ini'!$C$4,(('info ini'!$C$4-1)*L10/K10)+1)</f>
-        <v>0.0417137145996094</v>
+        <v>17.1661376953125</v>
       </c>
       <c r="G11" s="16" t="n">
         <f aca="false">F11*'info ini'!$C$6</f>
-        <v>0.0458850860595703</v>
+        <v>18.8827514648438</v>
       </c>
       <c r="H11" s="16" t="n">
         <f aca="false">I10*'info ini'!D$4</f>
-        <v>0.1473717306875</v>
+        <v>4.715895382</v>
       </c>
       <c r="I11" s="18" t="n">
         <f aca="false">IF(R10=1,'info ini'!$D$7,1)*I10*'info ini'!$D$4</f>
-        <v>0.1473717306875</v>
+        <v>4.715895382</v>
       </c>
       <c r="J11" s="16" t="n">
         <f aca="false">I11*'info ini'!$D$6</f>
-        <v>0.36842932671875</v>
+        <v>11.789738455</v>
       </c>
       <c r="K11" s="16" t="n">
         <f aca="false">J11+G11</f>
-        <v>0.414314412778321</v>
+        <v>30.6724899198438</v>
       </c>
       <c r="L11" s="18" t="n">
         <f aca="false">IF((G11+J11)&lt;B11,(G11+J11),B11)</f>
-        <v>0.414314412778321</v>
+        <v>17.729677550518</v>
       </c>
       <c r="M11" s="19" t="n">
         <f aca="false">IF(B11=0,0,L11/B11)</f>
-        <v>0.00163896518189666</v>
+        <v>1</v>
       </c>
       <c r="N11" s="16" t="n">
         <f aca="false">IF((N10-(B11/15))&gt;0,N10-(B11/15),0)</f>
-        <v>248.528703115632</v>
+        <v>52.287989565659</v>
       </c>
       <c r="O11" s="19" t="n">
         <f aca="false">A11*100/11</f>
@@ -4209,15 +4198,15 @@
       </c>
       <c r="P11" s="19" t="n">
         <f aca="false">N11/300</f>
-        <v>0.828429010385441</v>
+        <v>0.174293298552197</v>
       </c>
       <c r="Q11" s="19" t="n">
         <f aca="false">N11*O11*5/(100*300)</f>
-        <v>3.38902776975862</v>
+        <v>0.713018039531713</v>
       </c>
       <c r="R11" s="11" t="n">
         <f aca="false">BPH!C11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="16"/>
       <c r="T11" s="11" t="n">
@@ -4231,55 +4220,55 @@
       </c>
       <c r="B12" s="16" t="n">
         <f aca="false">C12+D12</f>
-        <v>418.349573783419</v>
+        <v>10</v>
       </c>
       <c r="C12" s="17" t="n">
         <f aca="false">C11*(1-M11)*IF(SUM($R$2:R11)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>391.848808525698</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="16" t="n">
         <f aca="false">D11*(1-M11)*IF(SUM($R$2,R11)=0,'info ini'!B$4,'info ini'!B$5)*IF(R11=1,'info ini'!B$7,1)+9.8</f>
-        <v>26.5007652577205</v>
+        <v>9.8</v>
       </c>
       <c r="E12" s="16" t="n">
         <f aca="false">F11*'info ini'!C$4</f>
-        <v>0.0521421432495117</v>
+        <v>21.4576721191406</v>
       </c>
       <c r="F12" s="18" t="n">
         <f aca="false">IF(R11=1,'info ini'!$C$7,1)*F11*IF(K11=L11,'info ini'!$C$4,(('info ini'!$C$4-1)*L11/K11)+1)</f>
-        <v>0.0156426429748535</v>
+        <v>19.6467814816585</v>
       </c>
       <c r="G12" s="16" t="n">
         <f aca="false">F12*'info ini'!$C$6</f>
-        <v>0.0172069072723389</v>
+        <v>21.6114596298244</v>
       </c>
       <c r="H12" s="16" t="n">
         <f aca="false">I11*'info ini'!D$4</f>
-        <v>0.16210890375625</v>
+        <v>5.18748492020001</v>
       </c>
       <c r="I12" s="18" t="n">
         <f aca="false">IF(R11=1,'info ini'!$D$7,1)*I11*'info ini'!$D$4</f>
-        <v>0.0810544518781251</v>
+        <v>5.18748492020001</v>
       </c>
       <c r="J12" s="16" t="n">
         <f aca="false">I12*'info ini'!$D$6</f>
-        <v>0.202636129695313</v>
+        <v>12.9687123005</v>
       </c>
       <c r="K12" s="16" t="n">
         <f aca="false">J12+G12</f>
-        <v>0.219843036967652</v>
+        <v>34.5801719303244</v>
       </c>
       <c r="L12" s="18" t="n">
         <f aca="false">IF((G12+J12)&lt;B12,(G12+J12),B12)</f>
-        <v>0.219843036967652</v>
+        <v>10</v>
       </c>
       <c r="M12" s="19" t="n">
         <f aca="false">IF(B12=0,0,L12/B12)</f>
-        <v>0.000525500803023323</v>
+        <v>1</v>
       </c>
       <c r="N12" s="16" t="n">
         <f aca="false">IF((N11-(B12/15))&gt;0,N11-(B12/15),0)</f>
-        <v>220.638731530071</v>
+        <v>51.6213228989923</v>
       </c>
       <c r="O12" s="19" t="n">
         <f aca="false">A12*100/11</f>
@@ -4287,11 +4276,11 @@
       </c>
       <c r="P12" s="19" t="n">
         <f aca="false">N12/300</f>
-        <v>0.73546243843357</v>
+        <v>0.172071076329974</v>
       </c>
       <c r="Q12" s="19" t="n">
         <f aca="false">N12*O12*5/(100*300)</f>
-        <v>3.34301108378896</v>
+        <v>0.782141256045338</v>
       </c>
       <c r="R12" s="11" t="n">
         <f aca="false">BPH!C12</f>
@@ -4309,55 +4298,55 @@
       </c>
       <c r="B13" s="16" t="n">
         <f aca="false">C13+D13</f>
-        <v>727.67088775234</v>
+        <v>10</v>
       </c>
       <c r="C13" s="17" t="n">
         <f aca="false">C12*(1-M12)*IF(SUM($R$2:R12)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>705.157204991878</v>
+        <v>0.2</v>
       </c>
       <c r="D13" s="16" t="n">
         <f aca="false">D12*(1-M12)*IF(SUM($R$2,R12)=0,'info ini'!B$4,'info ini'!B$5)*IF(R12=1,'info ini'!B$7,1)+9.8</f>
-        <v>22.5136827604625</v>
+        <v>9.8</v>
       </c>
       <c r="E13" s="16" t="n">
         <f aca="false">F12*'info ini'!C$4</f>
-        <v>0.0195533037185669</v>
+        <v>24.5584768520731</v>
       </c>
       <c r="F13" s="18" t="n">
         <f aca="false">IF(R12=1,'info ini'!$C$7,1)*F12*IF(K12=L12,'info ini'!$C$4,(('info ini'!$C$4-1)*L12/K12)+1)</f>
-        <v>0.00586599111557007</v>
+        <v>6.32014817640535</v>
       </c>
       <c r="G13" s="16" t="n">
         <f aca="false">F13*'info ini'!$C$6</f>
-        <v>0.00645259022712707</v>
+        <v>6.95216299404589</v>
       </c>
       <c r="H13" s="16" t="n">
         <f aca="false">I12*'info ini'!D$4</f>
-        <v>0.0891598970659376</v>
+        <v>5.70623341222001</v>
       </c>
       <c r="I13" s="18" t="n">
         <f aca="false">IF(R12=1,'info ini'!$D$7,1)*I12*'info ini'!$D$4</f>
-        <v>0.0445799485329688</v>
+        <v>2.85311670611</v>
       </c>
       <c r="J13" s="16" t="n">
         <f aca="false">I13*'info ini'!$D$6</f>
-        <v>0.111449871332422</v>
+        <v>7.13279176527501</v>
       </c>
       <c r="K13" s="16" t="n">
         <f aca="false">J13+G13</f>
-        <v>0.117902461559549</v>
+        <v>14.0849547593209</v>
       </c>
       <c r="L13" s="18" t="n">
         <f aca="false">IF((G13+J13)&lt;B13,(G13+J13),B13)</f>
-        <v>0.117902461559549</v>
+        <v>10</v>
       </c>
       <c r="M13" s="19" t="n">
         <f aca="false">IF(B13=0,0,L13/B13)</f>
-        <v>0.000162027179517558</v>
+        <v>1</v>
       </c>
       <c r="N13" s="16" t="n">
         <f aca="false">IF((N12-(B13/15))&gt;0,N12-(B13/15),0)</f>
-        <v>172.127339013248</v>
+        <v>50.9546562323256</v>
       </c>
       <c r="O13" s="19" t="n">
         <f aca="false">A13*100/11</f>
@@ -4365,11 +4354,11 @@
       </c>
       <c r="P13" s="19" t="n">
         <f aca="false">N13/300</f>
-        <v>0.573757796710828</v>
+        <v>0.169848854107752</v>
       </c>
       <c r="Q13" s="19" t="n">
         <f aca="false">N13*O13*5/(100*300)</f>
-        <v>2.86878898355414</v>
+        <v>0.849244270538761</v>
       </c>
       <c r="R13" s="11" t="n">
         <f aca="false">BPH!C13</f>
@@ -4387,66 +4376,66 @@
       </c>
       <c r="B14" s="16" t="n">
         <f aca="false">C14+D14</f>
-        <v>1289.88212741324</v>
+        <v>10</v>
       </c>
       <c r="C14" s="17" t="n">
         <f aca="false">C13*(1-M13)*IF(SUM($R$2:R13)&gt;1,'info ini'!B$12,'info ini'!B$11)+0.2</f>
-        <v>1269.27731064591</v>
+        <v>0.2</v>
       </c>
       <c r="D14" s="16" t="n">
         <f aca="false">D13*(1-M13)*IF(SUM($R$2,R13)=0,'info ini'!B$4,'info ini'!B$5)*IF(R13=1,'info ini'!B$7,1)+9.8</f>
-        <v>20.6048167673332</v>
+        <v>9.8</v>
       </c>
       <c r="E14" s="16" t="n">
         <f aca="false">F13*'info ini'!C$4</f>
-        <v>0.00733248889446258</v>
+        <v>7.90018522050669</v>
       </c>
       <c r="F14" s="18" t="n">
         <f aca="false">IF(R13=1,'info ini'!$C$7,1)*F13*IF(K13=L13,'info ini'!$C$4,(('info ini'!$C$4-1)*L13/K13)+1)</f>
-        <v>0.00219974666833877</v>
+        <v>2.2325816455006</v>
       </c>
       <c r="G14" s="16" t="n">
         <f aca="false">F14*'info ini'!$C$6</f>
-        <v>0.00241972133517265</v>
+        <v>2.45583981005066</v>
       </c>
       <c r="H14" s="16" t="n">
         <f aca="false">I13*'info ini'!D$4</f>
-        <v>0.0490379433862657</v>
+        <v>3.138428376721</v>
       </c>
       <c r="I14" s="18" t="n">
         <f aca="false">IF(R13=1,'info ini'!$D$7,1)*I13*'info ini'!$D$4</f>
-        <v>0.0245189716931328</v>
+        <v>1.5692141883605</v>
       </c>
       <c r="J14" s="16" t="n">
         <f aca="false">I14*'info ini'!$D$6</f>
-        <v>0.0612974292328321</v>
+        <v>3.92303547090125</v>
       </c>
       <c r="K14" s="16" t="n">
         <f aca="false">J14+G14</f>
-        <v>0.0637171505680048</v>
+        <v>6.37887528095192</v>
       </c>
       <c r="L14" s="18" t="n">
         <f aca="false">IF((G14+J14)&lt;B14,(G14+J14),B14)</f>
-        <v>0.0637171505680048</v>
+        <v>6.37887528095192</v>
       </c>
       <c r="M14" s="19" t="n">
         <f aca="false">IF(B14=0,0,L14/B14)</f>
-        <v>4.93976536412553E-005</v>
+        <v>0.637887528095191</v>
       </c>
       <c r="N14" s="16" t="n">
         <f aca="false">IF((N13-(B14/15))&gt;0,N13-(B14/15),0)</f>
-        <v>86.1351971856992</v>
+        <v>50.287989565659</v>
       </c>
       <c r="O14" s="19" t="n">
         <v>100</v>
       </c>
       <c r="P14" s="19" t="n">
         <f aca="false">N14/300</f>
-        <v>0.287117323952331</v>
+        <v>0.16762663188553</v>
       </c>
       <c r="Q14" s="19" t="n">
         <f aca="false">N14*O14*5/(100*300)</f>
-        <v>1.43558661976165</v>
+        <v>0.83813315942765</v>
       </c>
       <c r="R14" s="11" t="str">
         <f aca="false">BPH!C14</f>
@@ -4470,7 +4459,7 @@
       </c>
       <c r="R16" s="11" t="n">
         <f aca="false">SUM(R2:R15)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4638,6 +4627,227 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="11" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="60.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="11" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24" t="n">
+        <v>75</v>
+      </c>
+      <c r="C2" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="19" t="n">
+        <f aca="false">calcul!N3-calcul!N2</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19" t="n">
+        <f aca="false">IF(C3="","",calcul!N4-calcul!N3)</f>
+        <v>-6.66666666666667</v>
+      </c>
+      <c r="C4" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="n">
+        <f aca="false">IF(C4="","",calcul!N5-calcul!N4)</f>
+        <v>-7.35586766474728</v>
+      </c>
+      <c r="C5" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19" t="n">
+        <f aca="false">IF(C5="","",calcul!N6-calcul!N5)</f>
+        <v>-7.87789518081178</v>
+      </c>
+      <c r="C6" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="19" t="n">
+        <f aca="false">IF(C6="","",calcul!N7-calcul!N6)</f>
+        <v>-8.09064735409457</v>
+      </c>
+      <c r="C7" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="19" t="n">
+        <f aca="false">IF(C7="","",calcul!N8-calcul!N7)</f>
+        <v>-7.78367833945686</v>
+      </c>
+      <c r="C8" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="19" t="n">
+        <f aca="false">IF(C8="","",calcul!N9-calcul!N8)</f>
+        <v>-6.65000118516963</v>
+      </c>
+      <c r="C9" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="19" t="n">
+        <f aca="false">IF(C9="","",calcul!N10-calcul!N9)</f>
+        <v>-2.10527554002638</v>
+      </c>
+      <c r="C10" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="19" t="n">
+        <f aca="false">IF(C10="","",calcul!N11-calcul!N10)</f>
+        <v>-1.18197850336787</v>
+      </c>
+      <c r="C11" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="19" t="n">
+        <f aca="false">IF(C11="","",calcul!N12-calcul!N11)</f>
+        <v>-0.666666666666664</v>
+      </c>
+      <c r="C12" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="19" t="n">
+        <f aca="false">IF(C12="","",calcul!N13-calcul!N12)</f>
+        <v>-0.666666666666664</v>
+      </c>
+      <c r="C13" s="28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="19" t="n">
+        <f aca="false">IF(C13="","",calcul!N14-calcul!N13)</f>
+        <v>-0.666666666666664</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="16"/>
+    </row>
+    <row r="17" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="16" t="n">
+        <f aca="false">SUM(B2:B16)</f>
+        <v>25.287989565659</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="31" t="n">
+        <f aca="false">IF(B14="","",5*B17/B2)</f>
+        <v>1.68586597104393</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:J11"/>
@@ -4652,334 +4862,334 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I1" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J1" s="23" t="n">
+      <c r="A1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I1" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J1" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I2" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" s="23" t="n">
+      <c r="A2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="23" t="n">
+      <c r="A3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J4" s="23" t="n">
+      <c r="A4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I5" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" s="23" t="n">
+      <c r="A5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J6" s="23" t="n">
+      <c r="A6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J7" s="23" t="n">
+      <c r="A7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" s="23" t="n">
+      <c r="A8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I9" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" s="23" t="n">
+      <c r="A9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="I10" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J10" s="23" t="n">
+      <c r="A10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" s="32" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="24" t="n">
+      <c r="A11" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="33" t="n">
         <f aca="false">SUM(A1:J10)</f>
         <v>300</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="34"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10 G11">
@@ -5016,225 +5226,4 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E18"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="11" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="60.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="11" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27" t="n">
-        <v>75</v>
-      </c>
-      <c r="C2" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19" t="n">
-        <f aca="false">calcul!N3-calcul!N2</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="29" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="19" t="n">
-        <f aca="false">IF(C3="","",calcul!N4-calcul!N3)</f>
-        <v>-6.66666666666669</v>
-      </c>
-      <c r="C4" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="19" t="n">
-        <f aca="false">IF(C4="","",calcul!N5-calcul!N4)</f>
-        <v>-3.48534666666666</v>
-      </c>
-      <c r="C5" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="19" t="n">
-        <f aca="false">IF(C5="","",calcul!N6-calcul!N5)</f>
-        <v>-2.66729751210642</v>
-      </c>
-      <c r="C6" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="19" t="n">
-        <f aca="false">IF(C6="","",calcul!N7-calcul!N6)</f>
-        <v>-2.87037225364213</v>
-      </c>
-      <c r="C7" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="19" t="n">
-        <f aca="false">IF(C7="","",calcul!N8-calcul!N7)</f>
-        <v>-3.82953613343653</v>
-      </c>
-      <c r="C8" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" s="19" t="n">
-        <f aca="false">IF(C8="","",calcul!N9-calcul!N8)</f>
-        <v>-5.76720277724633</v>
-      </c>
-      <c r="C9" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" s="19" t="n">
-        <f aca="false">IF(C9="","",calcul!N10-calcul!N9)</f>
-        <v>-9.33219175663402</v>
-      </c>
-      <c r="C10" s="30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" s="19" t="n">
-        <f aca="false">IF(C10="","",calcul!N11-calcul!N10)</f>
-        <v>-16.8526831179686</v>
-      </c>
-      <c r="C11" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" s="19" t="n">
-        <f aca="false">IF(C11="","",calcul!N12-calcul!N11)</f>
-        <v>-27.8899715855613</v>
-      </c>
-      <c r="C12" s="30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="19" t="n">
-        <f aca="false">IF(C12="","",calcul!N13-calcul!N12)</f>
-        <v>-48.5113925168227</v>
-      </c>
-      <c r="C13" s="32" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="19" t="n">
-        <f aca="false">IF(C13="","",calcul!N14-calcul!N13)</f>
-        <v>-85.9921418275493</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="16"/>
-    </row>
-    <row r="17" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="16" t="n">
-        <f aca="false">SUM(B2:B16)</f>
-        <v>-138.864802814301</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="35" t="n">
-        <f aca="false">IF(B14="","",5*B17/B2)</f>
-        <v>-9.25765352095337</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>